<commit_message>
Created gitignore for no needed folders by default
</commit_message>
<xml_diff>
--- a/Predictions/PV_cp_cnn.xlsx
+++ b/Predictions/PV_cp_cnn.xlsx
@@ -483,1322 +483,1322 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5.653803825378418</v>
+        <v>7.228312492370605</v>
       </c>
       <c r="D2" t="n">
-        <v>-9.45506477355957</v>
+        <v>-5.794445037841797</v>
       </c>
       <c r="E2" t="n">
-        <v>-4.90446662902832</v>
+        <v>-0.2779783308506012</v>
       </c>
       <c r="F2" t="n">
-        <v>-9.836400032043457</v>
+        <v>-8.81078052520752</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.899656057357788</v>
+        <v>-1.111973762512207</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6799779534339905</v>
+        <v>-1.36834442615509</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.03955951504409314</v>
+        <v>0.07536812081933023</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1568202170729637</v>
+        <v>0.1138364183902741</v>
       </c>
       <c r="C3" t="n">
-        <v>6.982532501220703</v>
+        <v>4.650302410125732</v>
       </c>
       <c r="D3" t="n">
-        <v>-7.362154483795166</v>
+        <v>-7.117703437805176</v>
       </c>
       <c r="E3" t="n">
-        <v>-5.915628433227539</v>
+        <v>-1.537674903869629</v>
       </c>
       <c r="F3" t="n">
-        <v>-10.17363929748535</v>
+        <v>-9.675335884094238</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1271894425153732</v>
+        <v>1.554833292961121</v>
       </c>
       <c r="H3" t="n">
-        <v>-3.742504596710205</v>
+        <v>-1.911463260650635</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.0760839606821537</v>
+        <v>0.03255421958863736</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7650198936462402</v>
+        <v>0.04652358889579773</v>
       </c>
       <c r="C4" t="n">
-        <v>3.098288774490356</v>
+        <v>6.114776611328125</v>
       </c>
       <c r="D4" t="n">
-        <v>-7.170287609100342</v>
+        <v>-3.026534557342529</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.422814846038818</v>
+        <v>-2.383892059326172</v>
       </c>
       <c r="F4" t="n">
-        <v>-8.191237449645996</v>
+        <v>-9.164113998413086</v>
       </c>
       <c r="G4" t="n">
-        <v>3.839830875396729</v>
+        <v>5.175035953521729</v>
       </c>
       <c r="H4" t="n">
-        <v>-8.351227760314941</v>
+        <v>-7.086348056793213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.07078120946884156</v>
+        <v>0.1580563044548035</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.576290118694305</v>
+        <v>-0.2161237114667893</v>
       </c>
       <c r="C5" t="n">
-        <v>3.276397943496704</v>
+        <v>1.821904897689819</v>
       </c>
       <c r="D5" t="n">
-        <v>-4.016393184661865</v>
+        <v>-4.379329681396484</v>
       </c>
       <c r="E5" t="n">
-        <v>-5.721666812896729</v>
+        <v>-3.430261850357056</v>
       </c>
       <c r="F5" t="n">
-        <v>-6.446614265441895</v>
+        <v>-7.169382095336914</v>
       </c>
       <c r="G5" t="n">
-        <v>6.625461578369141</v>
+        <v>6.794341087341309</v>
       </c>
       <c r="H5" t="n">
-        <v>-8.255023956298828</v>
+        <v>-8.489947319030762</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.149731317460537</v>
+        <v>0.06525570601224899</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.888343858718872</v>
+        <v>-0.3636230206489563</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6246141791343689</v>
+        <v>4.996203422546387</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.865157127380371</v>
+        <v>-4.082178115844727</v>
       </c>
       <c r="E6" t="n">
-        <v>-4.726386070251465</v>
+        <v>-0.02229289337992668</v>
       </c>
       <c r="F6" t="n">
-        <v>-5.775547981262207</v>
+        <v>-6.049166679382324</v>
       </c>
       <c r="G6" t="n">
-        <v>12.28879928588867</v>
+        <v>8.814714431762695</v>
       </c>
       <c r="H6" t="n">
-        <v>-9.456803321838379</v>
+        <v>-10.54623985290527</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1488613161444664</v>
+        <v>0.2138410636782646</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7408175563812256</v>
+        <v>-0.4543855130672455</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6538363099098206</v>
+        <v>-0.0862443745136261</v>
       </c>
       <c r="D7" t="n">
-        <v>-7.128524303436279</v>
+        <v>-2.910331964492798</v>
       </c>
       <c r="E7" t="n">
-        <v>-5.34001350402832</v>
+        <v>1.411149978637695</v>
       </c>
       <c r="F7" t="n">
-        <v>-8.243284225463867</v>
+        <v>-5.359851360321045</v>
       </c>
       <c r="G7" t="n">
-        <v>11.89204502105713</v>
+        <v>10.24255752563477</v>
       </c>
       <c r="H7" t="n">
-        <v>-10.34447765350342</v>
+        <v>-12.00791549682617</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.08749550953507423</v>
+        <v>0.1569643959403038</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.7135080575943</v>
+        <v>-0.628906387090683</v>
       </c>
       <c r="C8" t="n">
-        <v>2.714996576309204</v>
+        <v>1.859254837036133</v>
       </c>
       <c r="D8" t="n">
-        <v>-4.651477813720703</v>
+        <v>-3.709414005279541</v>
       </c>
       <c r="E8" t="n">
-        <v>-3.041460037231445</v>
+        <v>2.289684295654297</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.850562691688538</v>
+        <v>-4.034414768218994</v>
       </c>
       <c r="G8" t="n">
-        <v>10.56995105743408</v>
+        <v>12.69857788085938</v>
       </c>
       <c r="H8" t="n">
-        <v>-11.51589393615723</v>
+        <v>-10.32339763641357</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.1338613751530647</v>
+        <v>0.1999437719583511</v>
       </c>
       <c r="B9" t="n">
-        <v>-4.032371563911438</v>
+        <v>-0.828288449048996</v>
       </c>
       <c r="C9" t="n">
-        <v>1.157655715942383</v>
+        <v>0.3891207873821259</v>
       </c>
       <c r="D9" t="n">
-        <v>-8.476902008056641</v>
+        <v>-4.748775482177734</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.8703367710113525</v>
+        <v>3.028037309646606</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.164852261543274</v>
+        <v>-2.520164728164673</v>
       </c>
       <c r="G9" t="n">
-        <v>17.68305778503418</v>
+        <v>10.12538623809814</v>
       </c>
       <c r="H9" t="n">
-        <v>-6.705341815948486</v>
+        <v>-5.853835105895996</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2425306838750839</v>
+        <v>0.2787930589914322</v>
       </c>
       <c r="B10" t="n">
-        <v>-4.553830766677857</v>
+        <v>-0.782946343421936</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.492339611053467</v>
+        <v>-2.307965040206909</v>
       </c>
       <c r="D10" t="n">
-        <v>-6.409841060638428</v>
+        <v>-2.97805643081665</v>
       </c>
       <c r="E10" t="n">
-        <v>1.015111923217773</v>
+        <v>3.011341571807861</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.04346291720867157</v>
+        <v>-2.864524602890015</v>
       </c>
       <c r="G10" t="n">
-        <v>13.41067504882812</v>
+        <v>12.56962871551514</v>
       </c>
       <c r="H10" t="n">
-        <v>-4.840447425842285</v>
+        <v>-5.307701110839844</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.244720171391964</v>
+        <v>0.2654033154249191</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.495678539276123</v>
+        <v>-1.044893441200256</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.565879583358765</v>
+        <v>-1.849961400032043</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.289535999298096</v>
+        <v>-6.708590984344482</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3835521340370178</v>
+        <v>4.705867290496826</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.1685182899236679</v>
+        <v>-0.875110387802124</v>
       </c>
       <c r="G11" t="n">
-        <v>16.39345359802246</v>
+        <v>11.23469066619873</v>
       </c>
       <c r="H11" t="n">
-        <v>-1.915578365325928</v>
+        <v>-2.561988353729248</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.3026859045028686</v>
+        <v>0.2073582744598389</v>
       </c>
       <c r="B12" t="n">
-        <v>-6.227140626907349</v>
+        <v>-1.036592099666596</v>
       </c>
       <c r="C12" t="n">
-        <v>-4.512838363647461</v>
+        <v>0.1355035006999969</v>
       </c>
       <c r="D12" t="n">
-        <v>-6.855685710906982</v>
+        <v>-5.757731437683105</v>
       </c>
       <c r="E12" t="n">
-        <v>2.22714900970459</v>
+        <v>4.075700759887695</v>
       </c>
       <c r="F12" t="n">
-        <v>3.554962158203125</v>
+        <v>-0.9381571412086487</v>
       </c>
       <c r="G12" t="n">
-        <v>16.55867767333984</v>
+        <v>10.3867073059082</v>
       </c>
       <c r="H12" t="n">
-        <v>-2.643069744110107</v>
+        <v>-1.91053295135498</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.2357800707221031</v>
+        <v>0.2550461614131928</v>
       </c>
       <c r="B13" t="n">
-        <v>-7.360333452224732</v>
+        <v>-1.307282426357269</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.265599489212036</v>
+        <v>-1.495688796043396</v>
       </c>
       <c r="D13" t="n">
-        <v>-2.806259632110596</v>
+        <v>-4.203418254852295</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1785293221473694</v>
+        <v>5.218381881713867</v>
       </c>
       <c r="F13" t="n">
-        <v>5.991874694824219</v>
+        <v>1.11765992641449</v>
       </c>
       <c r="G13" t="n">
-        <v>15.9516134262085</v>
+        <v>11.05342102050781</v>
       </c>
       <c r="H13" t="n">
-        <v>1.183537840843201</v>
+        <v>2.071201324462891</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.3643946492671967</v>
+        <v>0.2612629589438439</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.376822662353516</v>
+        <v>-1.086449556350708</v>
       </c>
       <c r="C14" t="n">
-        <v>-6.585517406463623</v>
+        <v>-1.708337903022766</v>
       </c>
       <c r="D14" t="n">
-        <v>-5.782844543457031</v>
+        <v>-4.360854625701904</v>
       </c>
       <c r="E14" t="n">
-        <v>3.989960670471191</v>
+        <v>6.152783870697021</v>
       </c>
       <c r="F14" t="n">
-        <v>6.027334213256836</v>
+        <v>-0.5595033168792725</v>
       </c>
       <c r="G14" t="n">
-        <v>12.59235954284668</v>
+        <v>6.175538539886475</v>
       </c>
       <c r="H14" t="n">
-        <v>0.04213961586356163</v>
+        <v>3.464868545532227</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.3006063675880432</v>
+        <v>0.3245542120933533</v>
       </c>
       <c r="B15" t="n">
-        <v>-7.597548503875733</v>
+        <v>-1.814876070022583</v>
       </c>
       <c r="C15" t="n">
-        <v>-4.442989826202393</v>
+        <v>-3.873251914978027</v>
       </c>
       <c r="D15" t="n">
-        <v>-4.515466213226318</v>
+        <v>-6.030617237091064</v>
       </c>
       <c r="E15" t="n">
-        <v>4.235147476196289</v>
+        <v>5.205160140991211</v>
       </c>
       <c r="F15" t="n">
-        <v>6.502001285552979</v>
+        <v>4.972690105438232</v>
       </c>
       <c r="G15" t="n">
-        <v>12.2869758605957</v>
+        <v>5.809774875640869</v>
       </c>
       <c r="H15" t="n">
-        <v>0.773665726184845</v>
+        <v>0.8549283742904663</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.3208064460754395</v>
+        <v>0.371340696811676</v>
       </c>
       <c r="B16" t="n">
-        <v>-6.547559900283813</v>
+        <v>-1.857650818824768</v>
       </c>
       <c r="C16" t="n">
-        <v>-5.121472358703613</v>
+        <v>-5.473609924316406</v>
       </c>
       <c r="D16" t="n">
-        <v>-7.078282833099365</v>
+        <v>-5.390738010406494</v>
       </c>
       <c r="E16" t="n">
-        <v>5.727447509765625</v>
+        <v>6.029065608978271</v>
       </c>
       <c r="F16" t="n">
-        <v>4.2440185546875</v>
+        <v>5.297551155090332</v>
       </c>
       <c r="G16" t="n">
-        <v>6.770132541656494</v>
+        <v>4.364377975463867</v>
       </c>
       <c r="H16" t="n">
-        <v>2.436364650726318</v>
+        <v>5.239752292633057</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.3284795796871186</v>
+        <v>0.3346324223279953</v>
       </c>
       <c r="B17" t="n">
-        <v>-7.392401561737061</v>
+        <v>-1.62575231552124</v>
       </c>
       <c r="C17" t="n">
-        <v>-5.379199504852295</v>
+        <v>-4.217981815338135</v>
       </c>
       <c r="D17" t="n">
-        <v>-4.869113445281982</v>
+        <v>-6.755410194396973</v>
       </c>
       <c r="E17" t="n">
-        <v>5.340146541595459</v>
+        <v>8.228316307067871</v>
       </c>
       <c r="F17" t="n">
-        <v>6.060836791992188</v>
+        <v>3.536346912384033</v>
       </c>
       <c r="G17" t="n">
-        <v>5.522574424743652</v>
+        <v>0.5608872771263123</v>
       </c>
       <c r="H17" t="n">
-        <v>0.8118055462837219</v>
+        <v>4.10211181640625</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.3895710784196854</v>
+        <v>0.4222528326511383</v>
       </c>
       <c r="B18" t="n">
-        <v>-7.376628570556641</v>
+        <v>-2.01890344619751</v>
       </c>
       <c r="C18" t="n">
-        <v>-7.431145191192627</v>
+        <v>-7.215089321136475</v>
       </c>
       <c r="D18" t="n">
-        <v>-4.544234275817871</v>
+        <v>-8.483136177062988</v>
       </c>
       <c r="E18" t="n">
-        <v>5.811061382293701</v>
+        <v>7.98446798324585</v>
       </c>
       <c r="F18" t="n">
-        <v>6.026916980743408</v>
+        <v>6.522220134735107</v>
       </c>
       <c r="G18" t="n">
-        <v>1.159028649330139</v>
+        <v>-3.338004350662231</v>
       </c>
       <c r="H18" t="n">
-        <v>2.008039474487305</v>
+        <v>2.188982486724854</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.345938048362732</v>
+        <v>0.357539866566658</v>
       </c>
       <c r="B19" t="n">
-        <v>-7.189318361282349</v>
+        <v>-1.812340619564057</v>
       </c>
       <c r="C19" t="n">
-        <v>-5.965595245361328</v>
+        <v>-5.001544952392578</v>
       </c>
       <c r="D19" t="n">
-        <v>-5.017333507537842</v>
+        <v>-5.75928783416748</v>
       </c>
       <c r="E19" t="n">
-        <v>7.390029907226562</v>
+        <v>4.960259914398193</v>
       </c>
       <c r="F19" t="n">
-        <v>5.624109745025635</v>
+        <v>4.953433036804199</v>
       </c>
       <c r="G19" t="n">
-        <v>2.51450514793396</v>
+        <v>-5.089957237243652</v>
       </c>
       <c r="H19" t="n">
-        <v>1.768268227577209</v>
+        <v>2.112699508666992</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.3840714317560196</v>
+        <v>0.4294594067335129</v>
       </c>
       <c r="B20" t="n">
-        <v>-6.799793815612794</v>
+        <v>-1.657804882526398</v>
       </c>
       <c r="C20" t="n">
-        <v>-7.24642276763916</v>
+        <v>-7.461594104766846</v>
       </c>
       <c r="D20" t="n">
-        <v>-6.374450206756592</v>
+        <v>-5.931394577026367</v>
       </c>
       <c r="E20" t="n">
-        <v>5.963458061218262</v>
+        <v>5.329039096832275</v>
       </c>
       <c r="F20" t="n">
-        <v>4.786443710327148</v>
+        <v>3.779778480529785</v>
       </c>
       <c r="G20" t="n">
-        <v>-3.265783548355103</v>
+        <v>-9.266704559326172</v>
       </c>
       <c r="H20" t="n">
-        <v>1.997541308403015</v>
+        <v>1.94640064239502</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.2890308326482773</v>
+        <v>0.4148256307840347</v>
       </c>
       <c r="B21" t="n">
-        <v>-7.633254823684693</v>
+        <v>-1.751311638355255</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.054190158843994</v>
+        <v>-6.961038112640381</v>
       </c>
       <c r="D21" t="n">
-        <v>-7.59557580947876</v>
+        <v>-7.235725879669189</v>
       </c>
       <c r="E21" t="n">
-        <v>7.018465995788574</v>
+        <v>7.636866092681885</v>
       </c>
       <c r="F21" t="n">
-        <v>6.578786849975586</v>
+        <v>4.489934921264648</v>
       </c>
       <c r="G21" t="n">
-        <v>-4.501266479492188</v>
+        <v>-9.690211296081543</v>
       </c>
       <c r="H21" t="n">
-        <v>2.374178409576416</v>
+        <v>1.161316871643066</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.3386340808868408</v>
+        <v>0.4212013441324234</v>
       </c>
       <c r="B22" t="n">
-        <v>-6.609446372985841</v>
+        <v>-1.833708534240723</v>
       </c>
       <c r="C22" t="n">
-        <v>-5.720269203186035</v>
+        <v>-7.179122924804688</v>
       </c>
       <c r="D22" t="n">
-        <v>-3.579771995544434</v>
+        <v>-5.82427453994751</v>
       </c>
       <c r="E22" t="n">
-        <v>7.549747943878174</v>
+        <v>4.19942569732666</v>
       </c>
       <c r="F22" t="n">
-        <v>4.377104759216309</v>
+        <v>5.115716457366943</v>
       </c>
       <c r="G22" t="n">
-        <v>-10.92592334747314</v>
+        <v>-11.59263610839844</v>
       </c>
       <c r="H22" t="n">
-        <v>1.854192852973938</v>
+        <v>0.1981057375669479</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.4411210888624191</v>
+        <v>0.4657585847377778</v>
       </c>
       <c r="B23" t="n">
-        <v>-5.940849161148072</v>
+        <v>-1.59283189535141</v>
       </c>
       <c r="C23" t="n">
-        <v>-9.162611961364746</v>
+        <v>-8.703228950500488</v>
       </c>
       <c r="D23" t="n">
-        <v>-4.251810073852539</v>
+        <v>-7.214507102966309</v>
       </c>
       <c r="E23" t="n">
-        <v>6.078746795654297</v>
+        <v>5.207459926605225</v>
       </c>
       <c r="F23" t="n">
-        <v>2.939297437667847</v>
+        <v>3.286325931549072</v>
       </c>
       <c r="G23" t="n">
-        <v>-9.47633171081543</v>
+        <v>-6.39112377166748</v>
       </c>
       <c r="H23" t="n">
-        <v>0.6368582844734192</v>
+        <v>1.137335658073425</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.4456500554084778</v>
+        <v>0.53</v>
       </c>
       <c r="B24" t="n">
-        <v>-6.180853271484375</v>
+        <v>-1.583214874267578</v>
       </c>
       <c r="C24" t="n">
-        <v>-9.314731597900391</v>
+        <v>-10.90064239501953</v>
       </c>
       <c r="D24" t="n">
-        <v>-4.079325199127197</v>
+        <v>-9.144157409667969</v>
       </c>
       <c r="E24" t="n">
-        <v>4.485651016235352</v>
+        <v>3.515982627868652</v>
       </c>
       <c r="F24" t="n">
-        <v>3.455422878265381</v>
+        <v>3.213288307189941</v>
       </c>
       <c r="G24" t="n">
-        <v>-9.130809783935547</v>
+        <v>-10.74576473236084</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1205405294895172</v>
+        <v>1.436156511306763</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.491607638001442</v>
+        <v>0.4223352837562561</v>
       </c>
       <c r="B25" t="n">
-        <v>-6.48880467414856</v>
+        <v>-1.681421532630921</v>
       </c>
       <c r="C25" t="n">
-        <v>-10.85835933685303</v>
+        <v>-7.217909336090088</v>
       </c>
       <c r="D25" t="n">
-        <v>-4.731420993804932</v>
+        <v>-5.234928607940674</v>
       </c>
       <c r="E25" t="n">
-        <v>3.573874473571777</v>
+        <v>1.553748726844788</v>
       </c>
       <c r="F25" t="n">
-        <v>4.117667198181152</v>
+        <v>3.959140300750732</v>
       </c>
       <c r="G25" t="n">
-        <v>-11.33881282806396</v>
+        <v>-8.197382926940918</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.8750782012939453</v>
+        <v>-1.876669406890869</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.4214950090646744</v>
+        <v>0.4993910855054856</v>
       </c>
       <c r="B26" t="n">
-        <v>-6.662927255630493</v>
+        <v>-1.893256933689118</v>
       </c>
       <c r="C26" t="n">
-        <v>-8.503409385681152</v>
+        <v>-9.85364818572998</v>
       </c>
       <c r="D26" t="n">
-        <v>-2.92297625541687</v>
+        <v>-4.927354335784912</v>
       </c>
       <c r="E26" t="n">
-        <v>4.289812564849854</v>
+        <v>1.278206825256348</v>
       </c>
       <c r="F26" t="n">
-        <v>4.492114067077637</v>
+        <v>5.56796932220459</v>
       </c>
       <c r="G26" t="n">
-        <v>-11.95578861236572</v>
+        <v>-8.976748466491699</v>
       </c>
       <c r="H26" t="n">
-        <v>0.03409799560904503</v>
+        <v>-2.002404689788818</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.53</v>
+        <v>0.4895886915922165</v>
       </c>
       <c r="B27" t="n">
-        <v>-6.60126368522644</v>
+        <v>-1.921651704311371</v>
       </c>
       <c r="C27" t="n">
-        <v>-12.14788627624512</v>
+        <v>-9.518351554870605</v>
       </c>
       <c r="D27" t="n">
-        <v>-2.128310680389404</v>
+        <v>-5.744802474975586</v>
       </c>
       <c r="E27" t="n">
-        <v>2.17871880531311</v>
+        <v>-0.5590262413024902</v>
       </c>
       <c r="F27" t="n">
-        <v>4.359508037567139</v>
+        <v>5.783620357513428</v>
       </c>
       <c r="G27" t="n">
-        <v>-11.91915321350098</v>
+        <v>-4.451342105865479</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.1532654166221619</v>
+        <v>-1.0870760679245</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.4611238217353821</v>
+        <v>0.5293366634845734</v>
       </c>
       <c r="B28" t="n">
-        <v>-7.341657676696777</v>
+        <v>-2.242750930786133</v>
       </c>
       <c r="C28" t="n">
-        <v>-9.834465980529785</v>
+        <v>-10.87795257568359</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4804942607879639</v>
+        <v>-2.23879599571228</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.681118369102478</v>
+        <v>-1.881641030311584</v>
       </c>
       <c r="F28" t="n">
-        <v>5.951713085174561</v>
+        <v>8.222277641296387</v>
       </c>
       <c r="G28" t="n">
-        <v>-9.12940788269043</v>
+        <v>-5.495316028594971</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.706722617149353</v>
+        <v>-4.673801898956299</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.3765462678670883</v>
+        <v>0.5288608479499817</v>
       </c>
       <c r="B29" t="n">
-        <v>-6.523819541931153</v>
+        <v>-1.929557912349701</v>
       </c>
       <c r="C29" t="n">
-        <v>-6.993666648864746</v>
+        <v>-10.86167812347412</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.3383738994598389</v>
+        <v>-2.683833837509155</v>
       </c>
       <c r="E29" t="n">
-        <v>-2.455382108688354</v>
+        <v>-4.134635448455811</v>
       </c>
       <c r="F29" t="n">
-        <v>4.192965507507324</v>
+        <v>5.843664646148682</v>
       </c>
       <c r="G29" t="n">
-        <v>-6.344018459320068</v>
+        <v>-2.244258165359497</v>
       </c>
       <c r="H29" t="n">
-        <v>-5.332154750823975</v>
+        <v>-3.180820941925049</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.3696409088373184</v>
+        <v>0.4927377235889435</v>
       </c>
       <c r="B30" t="n">
-        <v>-7.121702642440797</v>
+        <v>-1.703421256542206</v>
       </c>
       <c r="C30" t="n">
-        <v>-6.76172924041748</v>
+        <v>-9.626065254211426</v>
       </c>
       <c r="D30" t="n">
-        <v>3.226950407028198</v>
+        <v>-1.133121013641357</v>
       </c>
       <c r="E30" t="n">
-        <v>-7.505757331848145</v>
+        <v>-7.52944803237915</v>
       </c>
       <c r="F30" t="n">
-        <v>5.478703498840332</v>
+        <v>4.126221656799316</v>
       </c>
       <c r="G30" t="n">
-        <v>-7.42233943939209</v>
+        <v>-2.371614933013916</v>
       </c>
       <c r="H30" t="n">
-        <v>-2.978699445724487</v>
+        <v>-3.170746564865112</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2783848470449448</v>
+        <v>0.4475151562690735</v>
       </c>
       <c r="B31" t="n">
-        <v>-5.707650899887085</v>
+        <v>-1.942450737953186</v>
       </c>
       <c r="C31" t="n">
-        <v>-3.696612119674683</v>
+        <v>-8.079201698303223</v>
       </c>
       <c r="D31" t="n">
-        <v>1.489211082458496</v>
+        <v>-0.1031844615936279</v>
       </c>
       <c r="E31" t="n">
-        <v>-8.876958847045898</v>
+        <v>-12.06551647186279</v>
       </c>
       <c r="F31" t="n">
-        <v>2.437807559967041</v>
+        <v>5.941583156585693</v>
       </c>
       <c r="G31" t="n">
-        <v>-3.759764671325684</v>
+        <v>0.1195114031434059</v>
       </c>
       <c r="H31" t="n">
-        <v>-3.03329873085022</v>
+        <v>-0.4839966893196106</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.3707437318563461</v>
+        <v>0.3692361718416214</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.77438497543335</v>
+        <v>-1.686814150810242</v>
       </c>
       <c r="C32" t="n">
-        <v>-6.798770904541016</v>
+        <v>-5.401623725891113</v>
       </c>
       <c r="D32" t="n">
-        <v>6.546842098236084</v>
+        <v>8.460021018981934</v>
       </c>
       <c r="E32" t="n">
-        <v>-11.294677734375</v>
+        <v>-15.16560649871826</v>
       </c>
       <c r="F32" t="n">
-        <v>4.731802463531494</v>
+        <v>4.000095367431641</v>
       </c>
       <c r="G32" t="n">
-        <v>-2.677718639373779</v>
+        <v>0.1398295611143112</v>
       </c>
       <c r="H32" t="n">
-        <v>-4.939930438995361</v>
+        <v>-3.052057266235352</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.2245207720994949</v>
+        <v>0.468418185710907</v>
       </c>
       <c r="B33" t="n">
-        <v>-6.712632446289063</v>
+        <v>-1.713371493816376</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.887420892715454</v>
+        <v>-8.794201850891113</v>
       </c>
       <c r="D33" t="n">
-        <v>6.690071105957031</v>
+        <v>7.909018039703369</v>
       </c>
       <c r="E33" t="n">
-        <v>-11.49570274353027</v>
+        <v>-14.52505588531494</v>
       </c>
       <c r="F33" t="n">
-        <v>4.599004745483398</v>
+        <v>4.201790332794189</v>
       </c>
       <c r="G33" t="n">
-        <v>-5.09229040145874</v>
+        <v>0.8828971982002258</v>
       </c>
       <c r="H33" t="n">
-        <v>-2.373816728591919</v>
+        <v>0.3448257446289062</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.1530321574211121</v>
+        <v>0.326066700220108</v>
       </c>
       <c r="B34" t="n">
-        <v>-5.939880723953247</v>
+        <v>-1.36983747959137</v>
       </c>
       <c r="C34" t="n">
-        <v>0.5137457251548767</v>
+        <v>-3.924986362457275</v>
       </c>
       <c r="D34" t="n">
-        <v>9.677059173583984</v>
+        <v>6.153608322143555</v>
       </c>
       <c r="E34" t="n">
-        <v>-12.36382675170898</v>
+        <v>-15.3846607208252</v>
       </c>
       <c r="F34" t="n">
-        <v>2.937215328216553</v>
+        <v>1.592746734619141</v>
       </c>
       <c r="G34" t="n">
-        <v>-4.109493732452393</v>
+        <v>-0.3612797558307648</v>
       </c>
       <c r="H34" t="n">
-        <v>0.7524218559265137</v>
+        <v>1.108520030975342</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.5760446442309581</v>
+        <v>0.5950227178842504</v>
       </c>
       <c r="B35" t="n">
-        <v>67.12821872158977</v>
+        <v>8.855342908731643</v>
       </c>
       <c r="C35" t="n">
-        <v>-3.256949663162231</v>
+        <v>-3.665666580200195</v>
       </c>
       <c r="D35" t="n">
-        <v>9.320235252380371</v>
+        <v>11.11362266540527</v>
       </c>
       <c r="E35" t="n">
-        <v>-12.42622756958008</v>
+        <v>-12.79242420196533</v>
       </c>
       <c r="F35" t="n">
-        <v>1.024024367332458</v>
+        <v>4.531621932983398</v>
       </c>
       <c r="G35" t="n">
-        <v>-2.465534210205078</v>
+        <v>-3.008621215820312</v>
       </c>
       <c r="H35" t="n">
-        <v>0.166785255074501</v>
+        <v>1.883589744567871</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.9258429132933984</v>
+        <v>0.7624046279039651</v>
       </c>
       <c r="B36" t="n">
-        <v>-598.0477792531145</v>
+        <v>-14.98458341281871</v>
       </c>
       <c r="C36" t="n">
-        <v>2.539982080459595</v>
+        <v>-3.407731056213379</v>
       </c>
       <c r="D36" t="n">
-        <v>12.40510082244873</v>
+        <v>12.71925735473633</v>
       </c>
       <c r="E36" t="n">
-        <v>-7.936156749725342</v>
+        <v>-11.94880676269531</v>
       </c>
       <c r="F36" t="n">
-        <v>0.4885174036026001</v>
+        <v>-0.6200312376022339</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.672225475311279</v>
+        <v>2.670026540756226</v>
       </c>
       <c r="H36" t="n">
-        <v>-1.611362099647522</v>
+        <v>4.217447757720947</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.9854273361874343</v>
+        <v>0.9170946474485934</v>
       </c>
       <c r="B37" t="n">
-        <v>6025.956393897622</v>
+        <v>40.50541976792329</v>
       </c>
       <c r="C37" t="n">
-        <v>2.155580759048462</v>
+        <v>0.9024844765663147</v>
       </c>
       <c r="D37" t="n">
-        <v>12.78581237792969</v>
+        <v>13.43979549407959</v>
       </c>
       <c r="E37" t="n">
-        <v>-5.631823539733887</v>
+        <v>-10.51724624633789</v>
       </c>
       <c r="F37" t="n">
-        <v>1.626761674880981</v>
+        <v>1.137380957603455</v>
       </c>
       <c r="G37" t="n">
-        <v>-3.977789640426636</v>
+        <v>0.7999133467674255</v>
       </c>
       <c r="H37" t="n">
-        <v>0.4700658321380615</v>
+        <v>2.309535264968872</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.9994786432932744</v>
+        <v>0.9787145859392893</v>
       </c>
       <c r="B38" t="n">
-        <v>-49178.69888090814</v>
+        <v>-106.9516739153979</v>
       </c>
       <c r="C38" t="n">
-        <v>5.016924381256104</v>
+        <v>2.573819875717163</v>
       </c>
       <c r="D38" t="n">
-        <v>12.49951267242432</v>
+        <v>14.915358543396</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.9030991792678833</v>
+        <v>-6.284309387207031</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.5329524874687195</v>
+        <v>2.188395500183105</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.772716522216797</v>
+        <v>-1.803589224815369</v>
       </c>
       <c r="H38" t="n">
-        <v>1.688389897346497</v>
+        <v>3.970500469207764</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.9999257146760382</v>
+        <v>0.9979468311956392</v>
       </c>
       <c r="B39" t="n">
-        <v>433650.9197279753</v>
+        <v>212.6521538415099</v>
       </c>
       <c r="C39" t="n">
-        <v>3.117336511611938</v>
+        <v>5.479612350463867</v>
       </c>
       <c r="D39" t="n">
-        <v>11.91916275024414</v>
+        <v>14.30289649963379</v>
       </c>
       <c r="E39" t="n">
-        <v>2.331615924835205</v>
+        <v>-3.044485807418823</v>
       </c>
       <c r="F39" t="n">
-        <v>0.2135843187570572</v>
+        <v>-0.9188953638076782</v>
       </c>
       <c r="G39" t="n">
-        <v>-3.424475431442261</v>
+        <v>-7.411818027496338</v>
       </c>
       <c r="H39" t="n">
-        <v>1.144328236579895</v>
+        <v>2.538632392883301</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.999999749297701</v>
+        <v>0.9996459995648017</v>
       </c>
       <c r="B40" t="n">
-        <v>-3191328.746648094</v>
+        <v>-390.215602888904</v>
       </c>
       <c r="C40" t="n">
-        <v>5.593725681304932</v>
+        <v>4.102579116821289</v>
       </c>
       <c r="D40" t="n">
-        <v>11.59312152862549</v>
+        <v>9.230926513671875</v>
       </c>
       <c r="E40" t="n">
-        <v>1.168919086456299</v>
+        <v>0.1069190949201584</v>
       </c>
       <c r="F40" t="n">
-        <v>-1.448671698570251</v>
+        <v>-1.370643615722656</v>
       </c>
       <c r="G40" t="n">
-        <v>-3.680985927581787</v>
+        <v>-5.339004039764404</v>
       </c>
       <c r="H40" t="n">
-        <v>1.698674321174622</v>
+        <v>3.785541296005249</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.000000001762465</v>
+        <v>0.9999339407975442</v>
       </c>
       <c r="B41" t="n">
-        <v>19699683.16564975</v>
+        <v>507.9977188326129</v>
       </c>
       <c r="C41" t="n">
-        <v>5.778951644897461</v>
+        <v>3.845309972763062</v>
       </c>
       <c r="D41" t="n">
-        <v>10.50806140899658</v>
+        <v>13.17351531982422</v>
       </c>
       <c r="E41" t="n">
-        <v>6.034224510192871</v>
+        <v>2.27704644203186</v>
       </c>
       <c r="F41" t="n">
-        <v>-2.800826549530029</v>
+        <v>-3.594303607940674</v>
       </c>
       <c r="G41" t="n">
-        <v>-4.035259246826172</v>
+        <v>-9.653149604797363</v>
       </c>
       <c r="H41" t="n">
-        <v>3.173066854476929</v>
+        <v>2.839799165725708</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.9999999997511972</v>
+        <v>0.9999952383626939</v>
       </c>
       <c r="B42" t="n">
-        <v>-65333767.48886446</v>
+        <v>-263.4877011079259</v>
       </c>
       <c r="C42" t="n">
-        <v>8.166824340820312</v>
+        <v>5.921552658081055</v>
       </c>
       <c r="D42" t="n">
-        <v>8.219392776489258</v>
+        <v>7.725522518157959</v>
       </c>
       <c r="E42" t="n">
-        <v>5.934537410736084</v>
+        <v>1.950505375862122</v>
       </c>
       <c r="F42" t="n">
-        <v>-6.056411743164062</v>
+        <v>-6.710937023162842</v>
       </c>
       <c r="G42" t="n">
-        <v>-9.089858055114746</v>
+        <v>-8.184427261352539</v>
       </c>
       <c r="H42" t="n">
-        <v>3.366066932678223</v>
+        <v>1.648319125175476</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.9999999999789329</v>
+        <v>1.000000716670502</v>
       </c>
       <c r="B43" t="n">
-        <v>327212862.8340886</v>
+        <v>378.8398594753247</v>
       </c>
       <c r="C43" t="n">
-        <v>4.14646053314209</v>
+        <v>9.956888198852539</v>
       </c>
       <c r="D43" t="n">
-        <v>5.195571422576904</v>
+        <v>3.978744268417358</v>
       </c>
       <c r="E43" t="n">
-        <v>3.621502876281738</v>
+        <v>4.756276607513428</v>
       </c>
       <c r="F43" t="n">
-        <v>-4.128128528594971</v>
+        <v>-3.060490846633911</v>
       </c>
       <c r="G43" t="n">
-        <v>-5.493937492370605</v>
+        <v>-5.112500667572021</v>
       </c>
       <c r="H43" t="n">
-        <v>2.301235914230347</v>
+        <v>3.920912027359009</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.000000000001789</v>
+        <v>1.000000030789375</v>
       </c>
       <c r="B44" t="n">
-        <v>-629447671.9172032</v>
+        <v>-12.82270424953359</v>
       </c>
       <c r="C44" t="n">
-        <v>7.165080070495605</v>
+        <v>6.449461936950684</v>
       </c>
       <c r="D44" t="n">
-        <v>2.994858026504517</v>
+        <v>0.3268660306930542</v>
       </c>
       <c r="E44" t="n">
-        <v>3.516398429870605</v>
+        <v>5.691595077514648</v>
       </c>
       <c r="F44" t="n">
-        <v>-7.64389181137085</v>
+        <v>-8.663524627685547</v>
       </c>
       <c r="G44" t="n">
-        <v>-8.68282413482666</v>
+        <v>-11.23757839202881</v>
       </c>
       <c r="H44" t="n">
-        <v>3.219171047210693</v>
+        <v>2.740109920501709</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.9999999999998302</v>
+        <v>1.000000000281756</v>
       </c>
       <c r="B45" t="n">
-        <v>782869358.9793085</v>
+        <v>12.13597016420181</v>
       </c>
       <c r="C45" t="n">
-        <v>7.343530654907227</v>
+        <v>7.062413215637207</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.4419060945510864</v>
+        <v>-1.647126197814941</v>
       </c>
       <c r="E45" t="n">
-        <v>4.416713237762451</v>
+        <v>3.385728120803833</v>
       </c>
       <c r="F45" t="n">
-        <v>-8.418839454650879</v>
+        <v>-5.567963123321533</v>
       </c>
       <c r="G45" t="n">
-        <v>-9.380785942077637</v>
+        <v>-10.03358173370361</v>
       </c>
       <c r="H45" t="n">
-        <v>4.309469699859619</v>
+        <v>4.087451457977295</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1.000000000000019</v>
+        <v>0.9999999999664921</v>
       </c>
       <c r="B46" t="n">
-        <v>-1252752377.189279</v>
+        <v>2.44754251275333</v>
       </c>
       <c r="C46" t="n">
-        <v>7.628774642944336</v>
+        <v>9.384305000305176</v>
       </c>
       <c r="D46" t="n">
-        <v>0.2177721261978149</v>
+        <v>-3.758740425109863</v>
       </c>
       <c r="E46" t="n">
-        <v>3.417239189147949</v>
+        <v>3.51796555519104</v>
       </c>
       <c r="F46" t="n">
-        <v>-8.012555122375488</v>
+        <v>-9.33400821685791</v>
       </c>
       <c r="G46" t="n">
-        <v>-6.015175342559814</v>
+        <v>-9.896098136901855</v>
       </c>
       <c r="H46" t="n">
-        <v>5.042635440826416</v>
+        <v>4.088279247283936</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.9999999999999979</v>
+        <v>1.000000000003905</v>
       </c>
       <c r="B47" t="n">
-        <v>1936407098.723585</v>
+        <v>1.601946925094203</v>
       </c>
       <c r="C47" t="n">
-        <v>7.653347969055176</v>
+        <v>9.340998649597168</v>
       </c>
       <c r="D47" t="n">
-        <v>-4.840800285339355</v>
+        <v>-7.098080158233643</v>
       </c>
       <c r="E47" t="n">
-        <v>1.896527528762817</v>
+        <v>3.93381929397583</v>
       </c>
       <c r="F47" t="n">
-        <v>-8.074653625488281</v>
+        <v>-10.48462200164795</v>
       </c>
       <c r="G47" t="n">
-        <v>-11.17644691467285</v>
+        <v>-4.796414852142334</v>
       </c>
       <c r="H47" t="n">
-        <v>4.456645488739014</v>
+        <v>4.001474857330322</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>1.000000000000861</v>
       </c>
       <c r="B48" t="n">
-        <v>-537007727.6064098</v>
+        <v>0.6901489951853556</v>
       </c>
       <c r="C48" t="n">
-        <v>5.294293880462646</v>
+        <v>3.2303307056427</v>
       </c>
       <c r="D48" t="n">
-        <v>-8.936630249023438</v>
+        <v>-8.222044944763184</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.9915367364883423</v>
+        <v>-0.3330569565296173</v>
       </c>
       <c r="F48" t="n">
-        <v>-9.520320892333984</v>
+        <v>-6.738816738128662</v>
       </c>
       <c r="G48" t="n">
-        <v>-13.54607009887695</v>
+        <v>-9.195765495300293</v>
       </c>
       <c r="H48" t="n">
-        <v>4.707723617553711</v>
+        <v>3.716835260391235</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>1.000000000000087</v>
       </c>
       <c r="B49" t="n">
-        <v>172694985.3418977</v>
+        <v>0.9806778820693435</v>
       </c>
       <c r="C49" t="n">
-        <v>1.779324531555176</v>
+        <v>5.385818958282471</v>
       </c>
       <c r="D49" t="n">
-        <v>-11.2612771987915</v>
+        <v>-11.04417037963867</v>
       </c>
       <c r="E49" t="n">
-        <v>-0.5415372252464294</v>
+        <v>-0.5892403721809387</v>
       </c>
       <c r="F49" t="n">
-        <v>-9.469868659973145</v>
+        <v>-9.061789512634277</v>
       </c>
       <c r="G49" t="n">
-        <v>-7.548924446105957</v>
+        <v>-4.354310512542725</v>
       </c>
       <c r="H49" t="n">
-        <v>4.55206298828125</v>
+        <v>5.9588303565979</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>1.000000000000017</v>
       </c>
       <c r="B50" t="n">
-        <v>140791263.8711056</v>
+        <v>0.998168661564369</v>
       </c>
       <c r="C50" t="n">
-        <v>5.794784069061279</v>
+        <v>3.738742589950562</v>
       </c>
       <c r="D50" t="n">
-        <v>-10.01843070983887</v>
+        <v>-9.293888092041016</v>
       </c>
       <c r="E50" t="n">
-        <v>-2.490528345108032</v>
+        <v>-2.466341257095337</v>
       </c>
       <c r="F50" t="n">
-        <v>-10.76559734344482</v>
+        <v>-9.192286491394043</v>
       </c>
       <c r="G50" t="n">
-        <v>-6.033401966094971</v>
+        <v>-5.335946083068848</v>
       </c>
       <c r="H50" t="n">
-        <v>6.429047107696533</v>
+        <v>3.190438747406006</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>1.000000000000003</v>
       </c>
       <c r="B51" t="n">
-        <v>11656926.325853</v>
+        <v>0.998168661564369</v>
       </c>
       <c r="C51" t="n">
-        <v>4.51434326171875</v>
+        <v>3.881455183029175</v>
       </c>
       <c r="D51" t="n">
-        <v>-7.657394886016846</v>
+        <v>-8.441463470458984</v>
       </c>
       <c r="E51" t="n">
-        <v>-3.969679594039917</v>
+        <v>-0.4846278131008148</v>
       </c>
       <c r="F51" t="n">
-        <v>-9.930767059326172</v>
+        <v>-12.83598041534424</v>
       </c>
       <c r="G51" t="n">
-        <v>-4.862458229064941</v>
+        <v>-3.353863716125488</v>
       </c>
       <c r="H51" t="n">
-        <v>8.647357940673828</v>
+        <v>3.155097961425781</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="B52" t="n">
-        <v>11656926.325853</v>
+        <v>0.9994228308819822</v>
       </c>
       <c r="C52" t="n">
-        <v>3.838231801986694</v>
+        <v>2.419675827026367</v>
       </c>
       <c r="D52" t="n">
-        <v>-6.67451286315918</v>
+        <v>-8.407197952270508</v>
       </c>
       <c r="E52" t="n">
-        <v>-5.057930946350098</v>
+        <v>-0.8141533136367798</v>
       </c>
       <c r="F52" t="n">
-        <v>-10.97615623474121</v>
+        <v>-10.07937240600586</v>
       </c>
       <c r="G52" t="n">
-        <v>-5.308623790740967</v>
+        <v>-1.176482319831848</v>
       </c>
       <c r="H52" t="n">
-        <v>7.221131324768066</v>
+        <v>2.987604379653931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>